<commit_message>
data analysis means a lot for optimization.
</commit_message>
<xml_diff>
--- a/qr2019/data.xlsx
+++ b/qr2019/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mofrankhu/Developer/hashcode/qr2019/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36EA3876-E18B-A147-BA66-0D8B43949456}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A294D14-21EB-0C40-9D2F-280AE8690771}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1040" yWindow="460" windowWidth="24480" windowHeight="15000" activeTab="3" xr2:uid="{AA4465B1-416A-1446-8EC5-FAEC5F11DE18}"/>
+    <workbookView xWindow="1040" yWindow="460" windowWidth="24480" windowHeight="15000" activeTab="1" xr2:uid="{AA4465B1-416A-1446-8EC5-FAEC5F11DE18}"/>
   </bookViews>
   <sheets>
     <sheet name="e" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,10 @@
     <sheet name="c" sheetId="3" r:id="rId3"/>
     <sheet name="b" sheetId="4" r:id="rId4"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlchart.v1.0" hidden="1">e!$O$47:$O$61</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">e!$P$47:$P$61</definedName>
+  </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -28,9 +32,78 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="24">
   <si>
     <t># file a tag is in</t>
+  </si>
+  <si>
+    <t>0: 500667</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1: 2145259</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2: 4376978</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 3: 5892438</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 4: 6309150</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 5: 5058548</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 6: 3485211</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 7: 2085540</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 8: 1096274</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 9: 474204</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 10: 181713</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 11: 80717</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 12: 23289</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 13: 6408</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 14: 3204</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 4050954, 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 10804631, 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 14232426, 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 16117909, 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 16192770, 5</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 15104858, 6</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 13097335, 7</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 11472009, 8</t>
   </si>
 </sst>
 </file>
@@ -467,6 +540,335 @@
           </a:p>
         </c:txPr>
         <c:crossAx val="181610223"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t># file a tag is</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> in</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>b!$K$1:$L$1</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>240000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>b!$K$2:$L$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>600000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-8F5C-F246-A3C5-E9C58D212A9B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="236561743"/>
+        <c:axId val="225275199"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="236561743"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="225275199"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="225275199"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="236561743"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1977,6 +2379,331 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>e!$P$47:$P$61</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>500667</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2145259</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4376978</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5892438</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6309150</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5058548</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3485211</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2085540</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1096274</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>474204</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>181713</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>80717</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>23289</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>6408</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3204</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-8FD8-C64E-B81F-7C6317F555D5}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:axId val="879212239"/>
+        <c:axId val="879261327"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="879212239"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="879261327"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="879261327"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="879212239"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr rtl="0">
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
       <c:layout>
         <c:manualLayout>
           <c:layoutTarget val="inner"/>
@@ -2342,7 +3069,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -3085,7 +3812,391 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="5"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="6"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="7"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="8"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="1"/>
+            <c:leaderLines>
+              <c:spPr>
+                <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="35000"/>
+                      <a:lumOff val="65000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:round/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:leaderLines>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+            </c:extLst>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>d!$P$42:$P$50</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>4050954</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10804631</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>14232426</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16117909</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16192770</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>15104858</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>13097335</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>11472009</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5366208</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-D1EE-B34C-B4D1-6EE88CCEA96B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr rtl="0">
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -3438,7 +4549,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -3779,7 +4890,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -4180,336 +5291,47 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t># file a tag is</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> in</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:noFill/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>b!$K$1:$L$1</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>240000</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>b!$K$2:$L$2</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>600000</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-8F5C-F246-A3C5-E9C58D212A9B}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="236561743"/>
-        <c:axId val="225275199"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="236561743"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="225275199"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="225275199"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="236561743"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
 </file>
 
-<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/colors10.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -4829,6 +5651,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors9.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -5345,7 +6207,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style10.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -5861,7 +6723,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -6377,8 +7239,8 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -6405,8 +7267,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -6507,7 +7369,7 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="19050" cap="rnd">
+      <a:ln w="28575" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -6539,10 +7401,10 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="rnd">
@@ -6582,23 +7444,22 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
         </a:schemeClr>
       </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="65000"/>
             <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:downBar>
@@ -6703,8 +7564,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -6836,20 +7697,19 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -6863,17 +7723,6 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
@@ -6893,7 +7742,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -7409,7 +8258,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -7925,8 +8774,8 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="251">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -7953,8 +8802,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -7983,7 +8832,7 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:chartArea>
   <cs:dataLabel>
     <cs:lnRef idx="0"/>
@@ -8034,6 +8883,13 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
@@ -8044,18 +8900,25 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="25400">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -8090,7 +8953,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="rnd">
@@ -8411,6 +9274,511 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
@@ -8442,6 +9810,522 @@
 </file>
 
 <file path=xl/charts/style8.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style9.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -9031,6 +10915,108 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>196850</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>615950</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A9B078BF-71F4-3E40-8B96-853210291032}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>355600</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>444500</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="Rectangle 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{229EB070-389A-4242-A201-ED971D00C1C0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="17691100" y="10033000"/>
+          <a:ext cx="1739900" cy="1739900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="C00000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -9103,6 +11089,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>781050</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>31750</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>400050</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3A71A612-8311-484C-9D29-2B259DA2A6BA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -9562,10 +11584,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84D393DE-EC87-7D49-A58F-E2F5B9701002}">
-  <dimension ref="A1:O187"/>
+  <dimension ref="A1:AC187"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+    <sheetView topLeftCell="L35" workbookViewId="0">
+      <selection activeCell="Z50" sqref="Z50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9961,7 +11983,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="11:12" x14ac:dyDescent="0.2">
+    <row r="33" spans="11:29" x14ac:dyDescent="0.2">
       <c r="K33">
         <v>2990</v>
       </c>
@@ -9969,7 +11991,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="11:12" x14ac:dyDescent="0.2">
+    <row r="34" spans="11:29" x14ac:dyDescent="0.2">
       <c r="K34">
         <v>2991</v>
       </c>
@@ -9977,7 +11999,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="11:12" x14ac:dyDescent="0.2">
+    <row r="35" spans="11:29" x14ac:dyDescent="0.2">
       <c r="K35">
         <v>2992</v>
       </c>
@@ -9985,7 +12007,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="11:12" x14ac:dyDescent="0.2">
+    <row r="36" spans="11:29" x14ac:dyDescent="0.2">
       <c r="K36">
         <v>2993</v>
       </c>
@@ -9993,7 +12015,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="11:12" x14ac:dyDescent="0.2">
+    <row r="37" spans="11:29" x14ac:dyDescent="0.2">
       <c r="K37">
         <v>2994</v>
       </c>
@@ -10001,7 +12023,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="11:12" x14ac:dyDescent="0.2">
+    <row r="38" spans="11:29" x14ac:dyDescent="0.2">
       <c r="K38">
         <v>2995</v>
       </c>
@@ -10009,7 +12031,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="39" spans="11:12" x14ac:dyDescent="0.2">
+    <row r="39" spans="11:29" x14ac:dyDescent="0.2">
       <c r="K39">
         <v>2996</v>
       </c>
@@ -10017,7 +12039,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="11:12" x14ac:dyDescent="0.2">
+    <row r="40" spans="11:29" x14ac:dyDescent="0.2">
       <c r="K40">
         <v>2997</v>
       </c>
@@ -10025,7 +12047,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="11:12" x14ac:dyDescent="0.2">
+    <row r="41" spans="11:29" x14ac:dyDescent="0.2">
       <c r="K41">
         <v>2998</v>
       </c>
@@ -10033,15 +12055,60 @@
         <v>6</v>
       </c>
     </row>
-    <row r="42" spans="11:12" x14ac:dyDescent="0.2">
+    <row r="42" spans="11:29" x14ac:dyDescent="0.2">
       <c r="K42">
         <v>2999</v>
       </c>
       <c r="L42">
         <v>2</v>
       </c>
-    </row>
-    <row r="43" spans="11:12" x14ac:dyDescent="0.2">
+      <c r="O42" t="s">
+        <v>1</v>
+      </c>
+      <c r="P42" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q42" t="s">
+        <v>3</v>
+      </c>
+      <c r="R42" t="s">
+        <v>4</v>
+      </c>
+      <c r="S42" t="s">
+        <v>5</v>
+      </c>
+      <c r="T42" t="s">
+        <v>6</v>
+      </c>
+      <c r="U42" t="s">
+        <v>7</v>
+      </c>
+      <c r="V42" t="s">
+        <v>8</v>
+      </c>
+      <c r="W42" t="s">
+        <v>9</v>
+      </c>
+      <c r="X42" t="s">
+        <v>10</v>
+      </c>
+      <c r="Y42" t="s">
+        <v>11</v>
+      </c>
+      <c r="Z42" t="s">
+        <v>12</v>
+      </c>
+      <c r="AA42" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB42" t="s">
+        <v>14</v>
+      </c>
+      <c r="AC42" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="43" spans="11:29" x14ac:dyDescent="0.2">
       <c r="K43">
         <v>3000</v>
       </c>
@@ -10049,15 +12116,60 @@
         <v>3</v>
       </c>
     </row>
-    <row r="44" spans="11:12" x14ac:dyDescent="0.2">
+    <row r="44" spans="11:29" x14ac:dyDescent="0.2">
       <c r="K44">
         <v>3002</v>
       </c>
       <c r="L44">
         <v>4</v>
       </c>
-    </row>
-    <row r="45" spans="11:12" x14ac:dyDescent="0.2">
+      <c r="O44" t="s">
+        <v>1</v>
+      </c>
+      <c r="P44" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q44" t="s">
+        <v>3</v>
+      </c>
+      <c r="R44" t="s">
+        <v>4</v>
+      </c>
+      <c r="S44" t="s">
+        <v>5</v>
+      </c>
+      <c r="T44" t="s">
+        <v>6</v>
+      </c>
+      <c r="U44" t="s">
+        <v>7</v>
+      </c>
+      <c r="V44" t="s">
+        <v>8</v>
+      </c>
+      <c r="W44" t="s">
+        <v>9</v>
+      </c>
+      <c r="X44" t="s">
+        <v>10</v>
+      </c>
+      <c r="Y44" t="s">
+        <v>11</v>
+      </c>
+      <c r="Z44" t="s">
+        <v>12</v>
+      </c>
+      <c r="AA44" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB44" t="s">
+        <v>14</v>
+      </c>
+      <c r="AC44" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="45" spans="11:29" x14ac:dyDescent="0.2">
       <c r="K45">
         <v>3005</v>
       </c>
@@ -10065,7 +12177,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="11:12" x14ac:dyDescent="0.2">
+    <row r="46" spans="11:29" x14ac:dyDescent="0.2">
       <c r="K46">
         <v>3006</v>
       </c>
@@ -10073,135 +12185,233 @@
         <v>3</v>
       </c>
     </row>
-    <row r="47" spans="11:12" x14ac:dyDescent="0.2">
+    <row r="47" spans="11:29" x14ac:dyDescent="0.2">
       <c r="K47">
         <v>3007</v>
       </c>
       <c r="L47">
         <v>4</v>
       </c>
-    </row>
-    <row r="48" spans="11:12" x14ac:dyDescent="0.2">
+      <c r="O47">
+        <v>0</v>
+      </c>
+      <c r="P47">
+        <v>500667</v>
+      </c>
+    </row>
+    <row r="48" spans="11:29" x14ac:dyDescent="0.2">
       <c r="K48">
         <v>3008</v>
       </c>
       <c r="L48">
         <v>3</v>
       </c>
-    </row>
-    <row r="49" spans="11:12" x14ac:dyDescent="0.2">
+      <c r="O48">
+        <v>1</v>
+      </c>
+      <c r="P48">
+        <v>2145259</v>
+      </c>
+    </row>
+    <row r="49" spans="11:17" x14ac:dyDescent="0.2">
       <c r="K49">
         <v>3009</v>
       </c>
       <c r="L49">
         <v>2</v>
       </c>
-    </row>
-    <row r="50" spans="11:12" x14ac:dyDescent="0.2">
+      <c r="O49">
+        <v>2</v>
+      </c>
+      <c r="P49">
+        <v>4376978</v>
+      </c>
+    </row>
+    <row r="50" spans="11:17" x14ac:dyDescent="0.2">
       <c r="K50">
         <v>3010</v>
       </c>
       <c r="L50">
         <v>1</v>
       </c>
-    </row>
-    <row r="51" spans="11:12" x14ac:dyDescent="0.2">
+      <c r="O50">
+        <v>3</v>
+      </c>
+      <c r="P50">
+        <v>5892438</v>
+      </c>
+    </row>
+    <row r="51" spans="11:17" x14ac:dyDescent="0.2">
       <c r="K51">
         <v>3011</v>
       </c>
       <c r="L51">
         <v>2</v>
       </c>
-    </row>
-    <row r="52" spans="11:12" x14ac:dyDescent="0.2">
+      <c r="O51">
+        <v>4</v>
+      </c>
+      <c r="P51">
+        <v>6309150</v>
+      </c>
+    </row>
+    <row r="52" spans="11:17" x14ac:dyDescent="0.2">
       <c r="K52">
         <v>3012</v>
       </c>
       <c r="L52">
         <v>1</v>
       </c>
-    </row>
-    <row r="53" spans="11:12" x14ac:dyDescent="0.2">
+      <c r="O52">
+        <v>5</v>
+      </c>
+      <c r="P52">
+        <v>5058548</v>
+      </c>
+    </row>
+    <row r="53" spans="11:17" x14ac:dyDescent="0.2">
       <c r="K53">
         <v>3013</v>
       </c>
       <c r="L53">
         <v>5</v>
       </c>
-    </row>
-    <row r="54" spans="11:12" x14ac:dyDescent="0.2">
+      <c r="O53">
+        <v>6</v>
+      </c>
+      <c r="P53">
+        <v>3485211</v>
+      </c>
+    </row>
+    <row r="54" spans="11:17" x14ac:dyDescent="0.2">
       <c r="K54">
         <v>3014</v>
       </c>
       <c r="L54">
         <v>3</v>
       </c>
-    </row>
-    <row r="55" spans="11:12" x14ac:dyDescent="0.2">
+      <c r="O54">
+        <v>7</v>
+      </c>
+      <c r="P54">
+        <v>2085540</v>
+      </c>
+    </row>
+    <row r="55" spans="11:17" x14ac:dyDescent="0.2">
       <c r="K55">
         <v>3015</v>
       </c>
       <c r="L55">
         <v>3</v>
       </c>
-    </row>
-    <row r="56" spans="11:12" x14ac:dyDescent="0.2">
+      <c r="O55">
+        <v>8</v>
+      </c>
+      <c r="P55">
+        <v>1096274</v>
+      </c>
+    </row>
+    <row r="56" spans="11:17" x14ac:dyDescent="0.2">
       <c r="K56">
         <v>3016</v>
       </c>
       <c r="L56">
         <v>2</v>
       </c>
-    </row>
-    <row r="57" spans="11:12" x14ac:dyDescent="0.2">
+      <c r="O56">
+        <v>9</v>
+      </c>
+      <c r="P56">
+        <v>474204</v>
+      </c>
+    </row>
+    <row r="57" spans="11:17" x14ac:dyDescent="0.2">
       <c r="K57">
         <v>3017</v>
       </c>
       <c r="L57">
         <v>3</v>
       </c>
-    </row>
-    <row r="58" spans="11:12" x14ac:dyDescent="0.2">
+      <c r="O57">
+        <v>10</v>
+      </c>
+      <c r="P57">
+        <v>181713</v>
+      </c>
+    </row>
+    <row r="58" spans="11:17" x14ac:dyDescent="0.2">
       <c r="K58">
         <v>3018</v>
       </c>
       <c r="L58">
         <v>6</v>
       </c>
-    </row>
-    <row r="59" spans="11:12" x14ac:dyDescent="0.2">
+      <c r="O58">
+        <v>11</v>
+      </c>
+      <c r="P58">
+        <v>80717</v>
+      </c>
+    </row>
+    <row r="59" spans="11:17" x14ac:dyDescent="0.2">
       <c r="K59">
         <v>3020</v>
       </c>
       <c r="L59">
         <v>5</v>
       </c>
-    </row>
-    <row r="60" spans="11:12" x14ac:dyDescent="0.2">
+      <c r="O59">
+        <v>12</v>
+      </c>
+      <c r="P59">
+        <v>23289</v>
+      </c>
+    </row>
+    <row r="60" spans="11:17" x14ac:dyDescent="0.2">
       <c r="K60">
         <v>3021</v>
       </c>
       <c r="L60">
         <v>1</v>
       </c>
-    </row>
-    <row r="61" spans="11:12" x14ac:dyDescent="0.2">
+      <c r="O60">
+        <v>13</v>
+      </c>
+      <c r="P60">
+        <v>6408</v>
+      </c>
+    </row>
+    <row r="61" spans="11:17" x14ac:dyDescent="0.2">
       <c r="K61">
         <v>3022</v>
       </c>
       <c r="L61">
         <v>1</v>
       </c>
-    </row>
-    <row r="62" spans="11:12" x14ac:dyDescent="0.2">
+      <c r="O61">
+        <v>14</v>
+      </c>
+      <c r="P61">
+        <v>3204</v>
+      </c>
+    </row>
+    <row r="62" spans="11:17" x14ac:dyDescent="0.2">
       <c r="K62">
         <v>3023</v>
       </c>
       <c r="L62">
         <v>4</v>
       </c>
-    </row>
-    <row r="63" spans="11:12" x14ac:dyDescent="0.2">
+      <c r="P62">
+        <f>SUM(P47:P61)</f>
+        <v>31719600</v>
+      </c>
+      <c r="Q62">
+        <f>P62/1000</f>
+        <v>31719.599999999999</v>
+      </c>
+    </row>
+    <row r="63" spans="11:17" x14ac:dyDescent="0.2">
       <c r="K63">
         <v>3025</v>
       </c>
@@ -10209,7 +12419,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="64" spans="11:12" x14ac:dyDescent="0.2">
+    <row r="64" spans="11:17" x14ac:dyDescent="0.2">
       <c r="K64">
         <v>3026</v>
       </c>
@@ -11212,10 +13422,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12B8BD84-CBC3-AC41-917A-929C6FF4FD3E}">
-  <dimension ref="A1:R76"/>
+  <dimension ref="A1:Y76"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="N11" sqref="N11"/>
+    <sheetView tabSelected="1" topLeftCell="M27" workbookViewId="0">
+      <selection activeCell="R50" sqref="R50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11593,7 +13803,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="13:14" x14ac:dyDescent="0.2">
+    <row r="33" spans="13:25" x14ac:dyDescent="0.2">
       <c r="M33">
         <v>3908</v>
       </c>
@@ -11601,7 +13811,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="13:14" x14ac:dyDescent="0.2">
+    <row r="34" spans="13:25" x14ac:dyDescent="0.2">
       <c r="M34">
         <v>3909</v>
       </c>
@@ -11609,7 +13819,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="13:14" x14ac:dyDescent="0.2">
+    <row r="35" spans="13:25" x14ac:dyDescent="0.2">
       <c r="M35">
         <v>3911</v>
       </c>
@@ -11617,7 +13827,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="13:14" x14ac:dyDescent="0.2">
+    <row r="36" spans="13:25" x14ac:dyDescent="0.2">
       <c r="M36">
         <v>3912</v>
       </c>
@@ -11625,7 +13835,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="13:14" x14ac:dyDescent="0.2">
+    <row r="37" spans="13:25" x14ac:dyDescent="0.2">
       <c r="M37">
         <v>3915</v>
       </c>
@@ -11633,15 +13843,45 @@
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="13:14" x14ac:dyDescent="0.2">
+    <row r="38" spans="13:25" x14ac:dyDescent="0.2">
       <c r="M38">
         <v>3916</v>
       </c>
       <c r="N38">
         <v>1</v>
       </c>
-    </row>
-    <row r="39" spans="13:14" x14ac:dyDescent="0.2">
+      <c r="P38">
+        <v>0</v>
+      </c>
+      <c r="Q38" t="s">
+        <v>16</v>
+      </c>
+      <c r="R38" t="s">
+        <v>17</v>
+      </c>
+      <c r="S38" t="s">
+        <v>18</v>
+      </c>
+      <c r="T38" t="s">
+        <v>19</v>
+      </c>
+      <c r="U38" t="s">
+        <v>20</v>
+      </c>
+      <c r="V38" t="s">
+        <v>21</v>
+      </c>
+      <c r="W38" t="s">
+        <v>22</v>
+      </c>
+      <c r="X38" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y38">
+        <v>5366208</v>
+      </c>
+    </row>
+    <row r="39" spans="13:25" x14ac:dyDescent="0.2">
       <c r="M39">
         <v>3917</v>
       </c>
@@ -11649,7 +13889,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="13:14" x14ac:dyDescent="0.2">
+    <row r="40" spans="13:25" x14ac:dyDescent="0.2">
       <c r="M40">
         <v>3918</v>
       </c>
@@ -11657,7 +13897,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="13:14" x14ac:dyDescent="0.2">
+    <row r="41" spans="13:25" x14ac:dyDescent="0.2">
       <c r="M41">
         <v>3920</v>
       </c>
@@ -11665,87 +13905,181 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="13:14" x14ac:dyDescent="0.2">
+    <row r="42" spans="13:25" x14ac:dyDescent="0.2">
       <c r="M42">
         <v>3921</v>
       </c>
       <c r="N42">
         <v>1</v>
       </c>
-    </row>
-    <row r="43" spans="13:14" x14ac:dyDescent="0.2">
+      <c r="P42">
+        <v>4050954</v>
+      </c>
+      <c r="Q42">
+        <v>0</v>
+      </c>
+      <c r="R42">
+        <f t="shared" ref="R42:R49" si="0">P42/P43</f>
+        <v>0.37492756578174674</v>
+      </c>
+    </row>
+    <row r="43" spans="13:25" x14ac:dyDescent="0.2">
       <c r="M43">
         <v>3926</v>
       </c>
       <c r="N43">
         <v>1</v>
       </c>
-    </row>
-    <row r="44" spans="13:14" x14ac:dyDescent="0.2">
+      <c r="P43">
+        <v>10804631</v>
+      </c>
+      <c r="Q43">
+        <v>1</v>
+      </c>
+      <c r="R43">
+        <f t="shared" si="0"/>
+        <v>0.75915595837280303</v>
+      </c>
+    </row>
+    <row r="44" spans="13:25" x14ac:dyDescent="0.2">
       <c r="M44">
         <v>11002</v>
       </c>
       <c r="N44">
         <v>1</v>
       </c>
-    </row>
-    <row r="45" spans="13:14" x14ac:dyDescent="0.2">
+      <c r="P44">
+        <v>14232426</v>
+      </c>
+      <c r="Q44">
+        <v>2</v>
+      </c>
+      <c r="R44">
+        <f t="shared" si="0"/>
+        <v>0.88301937925074525</v>
+      </c>
+    </row>
+    <row r="45" spans="13:25" x14ac:dyDescent="0.2">
       <c r="M45">
         <v>17678</v>
       </c>
       <c r="N45">
         <v>1</v>
       </c>
-    </row>
-    <row r="46" spans="13:14" x14ac:dyDescent="0.2">
+      <c r="P45">
+        <v>16117909</v>
+      </c>
+      <c r="Q45">
+        <v>3</v>
+      </c>
+      <c r="R45">
+        <f t="shared" si="0"/>
+        <v>0.99537688733922614</v>
+      </c>
+    </row>
+    <row r="46" spans="13:25" x14ac:dyDescent="0.2">
       <c r="M46">
         <v>17681</v>
       </c>
       <c r="N46">
         <v>1</v>
       </c>
-    </row>
-    <row r="47" spans="13:14" x14ac:dyDescent="0.2">
+      <c r="P46">
+        <v>16192770</v>
+      </c>
+      <c r="Q46">
+        <v>4</v>
+      </c>
+      <c r="R46">
+        <f t="shared" si="0"/>
+        <v>1.0720239806292784</v>
+      </c>
+    </row>
+    <row r="47" spans="13:25" x14ac:dyDescent="0.2">
       <c r="M47">
         <v>17693</v>
       </c>
       <c r="N47">
         <v>1</v>
       </c>
-    </row>
-    <row r="48" spans="13:14" x14ac:dyDescent="0.2">
+      <c r="P47">
+        <v>15104858</v>
+      </c>
+      <c r="Q47">
+        <v>5</v>
+      </c>
+      <c r="R47">
+        <f t="shared" si="0"/>
+        <v>1.1532772125016273</v>
+      </c>
+    </row>
+    <row r="48" spans="13:25" x14ac:dyDescent="0.2">
       <c r="M48">
         <v>17700</v>
       </c>
       <c r="N48">
         <v>1</v>
       </c>
-    </row>
-    <row r="49" spans="13:14" x14ac:dyDescent="0.2">
+      <c r="P48">
+        <v>13097335</v>
+      </c>
+      <c r="Q48">
+        <v>6</v>
+      </c>
+      <c r="R48">
+        <f t="shared" si="0"/>
+        <v>1.1416775387815683</v>
+      </c>
+    </row>
+    <row r="49" spans="13:18" x14ac:dyDescent="0.2">
       <c r="M49">
         <v>17702</v>
       </c>
       <c r="N49">
         <v>1</v>
       </c>
-    </row>
-    <row r="50" spans="13:14" x14ac:dyDescent="0.2">
+      <c r="P49">
+        <v>11472009</v>
+      </c>
+      <c r="Q49">
+        <v>7</v>
+      </c>
+      <c r="R49">
+        <f t="shared" si="0"/>
+        <v>2.1378241395040969</v>
+      </c>
+    </row>
+    <row r="50" spans="13:18" x14ac:dyDescent="0.2">
       <c r="M50">
         <v>17706</v>
       </c>
       <c r="N50">
         <v>1</v>
       </c>
-    </row>
-    <row r="51" spans="13:14" x14ac:dyDescent="0.2">
+      <c r="P50">
+        <v>5366208</v>
+      </c>
+      <c r="Q50">
+        <v>8</v>
+      </c>
+      <c r="R50">
+        <f>P50/P51</f>
+        <v>5.0415758870565423E-2</v>
+      </c>
+    </row>
+    <row r="51" spans="13:18" x14ac:dyDescent="0.2">
       <c r="M51">
         <v>17710</v>
       </c>
       <c r="N51">
         <v>1</v>
       </c>
-    </row>
-    <row r="52" spans="13:14" x14ac:dyDescent="0.2">
+      <c r="P51">
+        <f>SUM(P42:P50)</f>
+        <v>106439100</v>
+      </c>
+    </row>
+    <row r="52" spans="13:18" x14ac:dyDescent="0.2">
       <c r="M52">
         <v>17717</v>
       </c>
@@ -11753,7 +14087,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="13:14" x14ac:dyDescent="0.2">
+    <row r="53" spans="13:18" x14ac:dyDescent="0.2">
       <c r="M53">
         <v>17722</v>
       </c>
@@ -11761,7 +14095,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="54" spans="13:14" x14ac:dyDescent="0.2">
+    <row r="54" spans="13:18" x14ac:dyDescent="0.2">
       <c r="M54">
         <v>17723</v>
       </c>
@@ -11769,7 +14103,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="13:14" x14ac:dyDescent="0.2">
+    <row r="55" spans="13:18" x14ac:dyDescent="0.2">
       <c r="M55">
         <v>17732</v>
       </c>
@@ -11777,7 +14111,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="13:14" x14ac:dyDescent="0.2">
+    <row r="56" spans="13:18" x14ac:dyDescent="0.2">
       <c r="M56">
         <v>17734</v>
       </c>
@@ -11785,7 +14119,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="13:14" x14ac:dyDescent="0.2">
+    <row r="57" spans="13:18" x14ac:dyDescent="0.2">
       <c r="M57">
         <v>17737</v>
       </c>
@@ -11793,7 +14127,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="13:14" x14ac:dyDescent="0.2">
+    <row r="58" spans="13:18" x14ac:dyDescent="0.2">
       <c r="M58">
         <v>17741</v>
       </c>
@@ -11801,7 +14135,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="13:14" x14ac:dyDescent="0.2">
+    <row r="59" spans="13:18" x14ac:dyDescent="0.2">
       <c r="M59">
         <v>17742</v>
       </c>
@@ -11809,7 +14143,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="13:14" x14ac:dyDescent="0.2">
+    <row r="60" spans="13:18" x14ac:dyDescent="0.2">
       <c r="M60">
         <v>17743</v>
       </c>
@@ -11817,7 +14151,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="13:14" x14ac:dyDescent="0.2">
+    <row r="61" spans="13:18" x14ac:dyDescent="0.2">
       <c r="M61">
         <v>17745</v>
       </c>
@@ -11825,7 +14159,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="13:14" x14ac:dyDescent="0.2">
+    <row r="62" spans="13:18" x14ac:dyDescent="0.2">
       <c r="M62">
         <v>17749</v>
       </c>
@@ -11833,7 +14167,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="63" spans="13:14" x14ac:dyDescent="0.2">
+    <row r="63" spans="13:18" x14ac:dyDescent="0.2">
       <c r="M63">
         <v>17761</v>
       </c>
@@ -11841,7 +14175,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="13:14" x14ac:dyDescent="0.2">
+    <row r="64" spans="13:18" x14ac:dyDescent="0.2">
       <c r="M64">
         <v>17762</v>
       </c>
@@ -12122,11 +14456,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54AA26B5-2E95-5445-8598-49A9947A5F92}">
   <dimension ref="A1:L14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="11" max="11" width="10.6640625" customWidth="1"/>
+    <col min="12" max="12" width="10.83203125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1">

</xml_diff>